<commit_message>
fix location to be travel location rather domicile
</commit_message>
<xml_diff>
--- a/Results/workday_tracker.xlsx
+++ b/Results/workday_tracker.xlsx
@@ -5084,7 +5084,7 @@
       </c>
       <c r="C114" s="8" t="inlineStr">
         <is>
-          <t>WFH SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D114" s="7" t="inlineStr"/>
@@ -9930,7 +9930,7 @@
       </c>
       <c r="C240" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D240" s="7" t="inlineStr"/>
@@ -9967,7 +9967,7 @@
       </c>
       <c r="C241" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA area</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D241" s="20" t="inlineStr"/>
@@ -10004,7 +10004,7 @@
       </c>
       <c r="C242" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA area</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D242" s="20" t="inlineStr"/>
@@ -10041,7 +10041,7 @@
       </c>
       <c r="C243" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA area</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D243" s="20" t="inlineStr"/>
@@ -10078,7 +10078,7 @@
       </c>
       <c r="C244" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA area</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D244" s="20" t="inlineStr"/>
@@ -10115,7 +10115,7 @@
       </c>
       <c r="C245" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA area</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D245" s="20" t="inlineStr"/>
@@ -12758,7 +12758,7 @@
       </c>
       <c r="C314" s="21" t="inlineStr">
         <is>
-          <t>vacation SFO</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="D314" s="20" t="inlineStr"/>
@@ -12832,7 +12832,7 @@
       </c>
       <c r="C316" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="D316" s="7" t="inlineStr"/>
@@ -14212,7 +14212,7 @@
       </c>
       <c r="C352" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D352" s="7" t="inlineStr"/>
@@ -14249,7 +14249,7 @@
       </c>
       <c r="C353" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D353" s="20" t="inlineStr"/>
@@ -14286,7 +14286,7 @@
       </c>
       <c r="C354" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D354" s="20" t="inlineStr"/>
@@ -14323,7 +14323,7 @@
       </c>
       <c r="C355" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D355" s="20" t="inlineStr"/>
@@ -14360,7 +14360,7 @@
       </c>
       <c r="C356" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D356" s="20" t="inlineStr"/>
@@ -14397,7 +14397,7 @@
       </c>
       <c r="C357" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D357" s="20" t="inlineStr"/>
@@ -14434,7 +14434,7 @@
       </c>
       <c r="C358" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D358" s="7" t="inlineStr"/>
@@ -14471,7 +14471,7 @@
       </c>
       <c r="C359" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D359" s="7" t="inlineStr"/>
@@ -14545,7 +14545,7 @@
       </c>
       <c r="C361" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D361" s="20" t="inlineStr"/>
@@ -14582,7 +14582,7 @@
       </c>
       <c r="C362" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D362" s="20" t="inlineStr"/>
@@ -14619,7 +14619,7 @@
       </c>
       <c r="C363" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D363" s="20" t="inlineStr"/>
@@ -14656,7 +14656,7 @@
       </c>
       <c r="C364" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D364" s="20" t="inlineStr"/>
@@ -19028,7 +19028,7 @@
       </c>
       <c r="C478" s="8" t="inlineStr">
         <is>
-          <t>WFH SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D478" s="7" t="inlineStr"/>
@@ -20650,7 +20650,7 @@
       </c>
       <c r="C520" s="8" t="inlineStr">
         <is>
-          <t>WFH SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D520" s="7" t="inlineStr"/>
@@ -24153,7 +24153,7 @@
       </c>
       <c r="C611" s="8" t="inlineStr">
         <is>
-          <t>WFH SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D611" s="7" t="inlineStr"/>
@@ -24391,7 +24391,7 @@
       </c>
       <c r="C617" s="8" t="inlineStr">
         <is>
-          <t>WFH SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D617" s="7" t="inlineStr"/>
@@ -24428,7 +24428,7 @@
       </c>
       <c r="C618" s="8" t="inlineStr">
         <is>
-          <t>WFH SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D618" s="7" t="inlineStr"/>
@@ -26806,7 +26806,7 @@
       </c>
       <c r="C680" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="D680" s="7" t="inlineStr"/>
@@ -26843,7 +26843,7 @@
       </c>
       <c r="C681" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="D681" s="7" t="inlineStr"/>
@@ -27625,7 +27625,7 @@
       </c>
       <c r="C701" s="8" t="inlineStr">
         <is>
-          <t>WFH SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D701" s="7" t="inlineStr"/>
@@ -28200,7 +28200,7 @@
       </c>
       <c r="C716" s="8" t="inlineStr">
         <is>
-          <t>WFH SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D716" s="7" t="inlineStr"/>
@@ -28442,7 +28442,7 @@
       </c>
       <c r="C722" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D722" s="7" t="inlineStr"/>
@@ -28479,7 +28479,7 @@
       </c>
       <c r="C723" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D723" s="7" t="inlineStr"/>
@@ -28516,7 +28516,7 @@
       </c>
       <c r="C724" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D724" s="20" t="inlineStr"/>
@@ -28553,7 +28553,7 @@
       </c>
       <c r="C725" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D725" s="20" t="inlineStr"/>
@@ -28627,7 +28627,7 @@
       </c>
       <c r="C727" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D727" s="20" t="inlineStr"/>
@@ -28664,7 +28664,7 @@
       </c>
       <c r="C728" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D728" s="20" t="inlineStr"/>
@@ -28701,7 +28701,7 @@
       </c>
       <c r="C729" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D729" s="7" t="inlineStr"/>
@@ -28738,7 +28738,7 @@
       </c>
       <c r="C730" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D730" s="7" t="inlineStr"/>
@@ -28775,7 +28775,7 @@
       </c>
       <c r="C731" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D731" s="20" t="inlineStr"/>
@@ -28812,7 +28812,7 @@
       </c>
       <c r="C732" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D732" s="20" t="inlineStr"/>
@@ -28886,7 +28886,7 @@
       </c>
       <c r="C734" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D734" s="20" t="inlineStr"/>
@@ -28923,7 +28923,7 @@
       </c>
       <c r="C735" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D735" s="20" t="inlineStr"/>
@@ -28960,7 +28960,7 @@
       </c>
       <c r="C736" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D736" s="7" t="inlineStr"/>
@@ -28997,7 +28997,7 @@
       </c>
       <c r="C737" s="8" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D737" s="7" t="inlineStr"/>
@@ -32844,7 +32844,7 @@
       </c>
       <c r="C840" s="21" t="inlineStr">
         <is>
-          <t>vacation (gf visit)</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D840" s="20" t="inlineStr"/>
@@ -32949,7 +32949,7 @@
       </c>
       <c r="C843" s="21" t="inlineStr">
         <is>
-          <t>vacation (gf visit)</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D843" s="20" t="inlineStr"/>
@@ -32984,7 +32984,7 @@
       </c>
       <c r="C844" s="21" t="inlineStr">
         <is>
-          <t>vacation (gf visit)</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D844" s="20" t="inlineStr"/>
@@ -33019,7 +33019,7 @@
       </c>
       <c r="C845" s="21" t="inlineStr">
         <is>
-          <t>vacation (gf visit)</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D845" s="20" t="inlineStr"/>
@@ -36474,7 +36474,7 @@
       </c>
       <c r="C944" s="21" t="inlineStr">
         <is>
-          <t>vacation PDX</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="D944" s="20" t="inlineStr"/>
@@ -36507,7 +36507,7 @@
       </c>
       <c r="C945" s="21" t="inlineStr">
         <is>
-          <t>vacation PDX</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="D945" s="20" t="inlineStr"/>
@@ -36540,7 +36540,7 @@
       </c>
       <c r="C946" s="8" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="D946" s="7" t="inlineStr"/>
@@ -39684,7 +39684,7 @@
       </c>
       <c r="C1042" s="21" t="inlineStr">
         <is>
-          <t>vacation SJC</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="D1042" s="20" t="inlineStr"/>
@@ -39715,7 +39715,7 @@
       </c>
       <c r="C1043" s="21" t="inlineStr">
         <is>
-          <t>vacation SJC</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="D1043" s="20" t="inlineStr"/>
@@ -39746,7 +39746,7 @@
       </c>
       <c r="C1044" s="8" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="D1044" s="7" t="inlineStr"/>
@@ -41104,7 +41104,7 @@
       </c>
       <c r="C1088" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D1088" s="20" t="inlineStr"/>
@@ -41133,7 +41133,7 @@
       </c>
       <c r="C1089" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D1089" s="20" t="inlineStr"/>
@@ -41162,7 +41162,7 @@
       </c>
       <c r="C1090" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D1090" s="20" t="inlineStr"/>
@@ -41220,7 +41220,7 @@
       </c>
       <c r="C1092" s="21" t="inlineStr">
         <is>
-          <t>vacation SEA</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D1092" s="20" t="inlineStr"/>
@@ -41336,7 +41336,7 @@
       </c>
       <c r="C1096" s="21" t="inlineStr">
         <is>
-          <t>vacation SFO</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="D1096" s="20" t="inlineStr"/>
@@ -41365,7 +41365,7 @@
       </c>
       <c r="C1097" s="21" t="inlineStr">
         <is>
-          <t>vacation SFO</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="D1097" s="20" t="inlineStr"/>

</xml_diff>